<commit_message>
base goa mods ATF/Pollock are good
may have to adjust env data/cindex if things dont work
</commit_message>
<xml_diff>
--- a/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_biomass_estimate.xlsx
+++ b/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_biomass_estimate.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/RceattleRuns/GOA/Model runs/GOA_18.5.1/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\RceattleRuns\GOA\Model runs\GOA_18.5.1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36786BAD-6D18-F042-9F0D-2A174BF4A3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13380" activeTab="2" xr2:uid="{56F0221B-99D3-5943-A98A-121E995483AB}"/>
+    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="1" r:id="rId1"/>
     <sheet name="SSB" sheetId="2" r:id="rId2"/>
     <sheet name="R" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>2018_Cod</t>
   </si>
@@ -46,11 +45,14 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>2020_Cod</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -118,8 +120,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 6" xfId="1" xr:uid="{FEC48C9C-EFE6-324F-A7C1-E548573F95BD}"/>
-    <cellStyle name="Normal_biom&amp;recr plots" xfId="2" xr:uid="{455DE5A1-A937-1045-997F-B9A2E427E301}"/>
+    <cellStyle name="Normal 6" xfId="1"/>
+    <cellStyle name="Normal_biom&amp;recr plots" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -430,20 +432,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D28FB5A-2205-7040-9D6F-3CDF6ADA5BB5}">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D43"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -456,8 +458,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1977</v>
       </c>
@@ -465,13 +470,16 @@
         <v>746.19600000000003</v>
       </c>
       <c r="C2">
-        <v>294.20999999999998</v>
+        <v>403588</v>
       </c>
       <c r="D2">
         <v>820.92700000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>364209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1978</v>
       </c>
@@ -479,13 +487,16 @@
         <v>964.72400000000005</v>
       </c>
       <c r="C3">
-        <v>319.51400000000001</v>
+        <v>422439</v>
       </c>
       <c r="D3">
         <v>880.01499999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>405023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1979</v>
       </c>
@@ -493,13 +504,16 @@
         <v>1346.35</v>
       </c>
       <c r="C4">
-        <v>373.34899999999999</v>
+        <v>504136</v>
       </c>
       <c r="D4">
         <v>951.24300000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>471526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1980</v>
       </c>
@@ -507,13 +521,16 @@
         <v>1812.05</v>
       </c>
       <c r="C5">
-        <v>429.50900000000001</v>
+        <v>593197</v>
       </c>
       <c r="D5">
         <v>1025</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>530446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1981</v>
       </c>
@@ -521,13 +538,16 @@
         <v>2831.55</v>
       </c>
       <c r="C6">
-        <v>459.70299999999997</v>
+        <v>635060</v>
       </c>
       <c r="D6">
         <v>1091</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>556366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1982</v>
       </c>
@@ -535,13 +555,16 @@
         <v>2955.59</v>
       </c>
       <c r="C7">
-        <v>481.92200000000003</v>
+        <v>668967</v>
       </c>
       <c r="D7">
         <v>1149</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>579603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1983</v>
       </c>
@@ -549,13 +572,16 @@
         <v>2690.68</v>
       </c>
       <c r="C8">
-        <v>505.71499999999997</v>
+        <v>713828</v>
       </c>
       <c r="D8">
         <v>1201</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>618424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1984</v>
       </c>
@@ -563,13 +589,16 @@
         <v>2390.54</v>
       </c>
       <c r="C9">
-        <v>526.43200000000002</v>
+        <v>758519</v>
       </c>
       <c r="D9">
         <v>1253</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>651063</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1985</v>
       </c>
@@ -577,13 +606,16 @@
         <v>1929.54</v>
       </c>
       <c r="C10">
-        <v>567.154</v>
+        <v>798787</v>
       </c>
       <c r="D10">
         <v>1321</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>690522</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1986</v>
       </c>
@@ -591,13 +623,16 @@
         <v>1622.15</v>
       </c>
       <c r="C11">
-        <v>623.23900000000003</v>
+        <v>837433</v>
       </c>
       <c r="D11">
         <v>1389</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>742523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1987</v>
       </c>
@@ -605,13 +640,16 @@
         <v>1965.93</v>
       </c>
       <c r="C12">
-        <v>665.81500000000005</v>
+        <v>871227</v>
       </c>
       <c r="D12">
         <v>1459</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>787267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1988</v>
       </c>
@@ -619,13 +657,16 @@
         <v>1863.57</v>
       </c>
       <c r="C13">
-        <v>683.11800000000005</v>
+        <v>873994</v>
       </c>
       <c r="D13">
         <v>1532</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>794280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1989</v>
       </c>
@@ -633,13 +674,16 @@
         <v>1647.42</v>
       </c>
       <c r="C14">
-        <v>681.07299999999998</v>
+        <v>857974</v>
       </c>
       <c r="D14">
         <v>1600</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>787561</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1990</v>
       </c>
@@ -647,13 +691,16 @@
         <v>1525.24</v>
       </c>
       <c r="C15">
-        <v>658.39499999999998</v>
+        <v>823846</v>
       </c>
       <c r="D15">
         <v>1660</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>769439</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1991</v>
       </c>
@@ -661,13 +708,16 @@
         <v>1839.76</v>
       </c>
       <c r="C16">
-        <v>617.68700000000001</v>
+        <v>776061</v>
       </c>
       <c r="D16">
         <v>1713</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>736250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1992</v>
       </c>
@@ -675,13 +725,16 @@
         <v>1921.6200000000003</v>
       </c>
       <c r="C17">
-        <v>589.08199999999999</v>
+        <v>743411</v>
       </c>
       <c r="D17">
         <v>1755</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>707463</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1993</v>
       </c>
@@ -689,13 +742,16 @@
         <v>1808.52</v>
       </c>
       <c r="C18">
-        <v>555.78200000000004</v>
+        <v>705219</v>
       </c>
       <c r="D18">
         <v>1773</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>665035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1994</v>
       </c>
@@ -703,13 +759,16 @@
         <v>1532.77</v>
       </c>
       <c r="C19">
-        <v>529.40700000000004</v>
+        <v>667998</v>
       </c>
       <c r="D19">
         <v>1782</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>628624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1995</v>
       </c>
@@ -717,13 +776,16 @@
         <v>1251.9100000000001</v>
       </c>
       <c r="C20">
-        <v>497.04500000000002</v>
+        <v>613486</v>
       </c>
       <c r="D20">
         <v>1776</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>585143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1996</v>
       </c>
@@ -731,13 +793,16 @@
         <v>1051.92</v>
       </c>
       <c r="C21">
-        <v>442.38400000000001</v>
+        <v>533819</v>
       </c>
       <c r="D21">
         <v>1770</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>519793</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1997</v>
       </c>
@@ -745,13 +810,16 @@
         <v>1073.49</v>
       </c>
       <c r="C22">
-        <v>395.96199999999999</v>
+        <v>470311</v>
       </c>
       <c r="D22">
         <v>1769</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>465313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1998</v>
       </c>
@@ -759,13 +827,16 @@
         <v>1032.3800000000001</v>
       </c>
       <c r="C23">
-        <v>356.73200000000003</v>
+        <v>418822</v>
       </c>
       <c r="D23">
         <v>1793</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>416933</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1999</v>
       </c>
@@ -773,13 +844,16 @@
         <v>769.31700000000001</v>
       </c>
       <c r="C24">
-        <v>326.392</v>
+        <v>379079</v>
       </c>
       <c r="D24">
         <v>1835</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>377406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2000</v>
       </c>
@@ -787,13 +861,16 @@
         <v>680.83900000000006</v>
       </c>
       <c r="C25">
-        <v>298.17899999999997</v>
+        <v>338390</v>
       </c>
       <c r="D25">
         <v>1906</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>338761</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2001</v>
       </c>
@@ -801,13 +878,16 @@
         <v>651.16600000000005</v>
       </c>
       <c r="C26">
-        <v>293.92899999999997</v>
+        <v>325728</v>
       </c>
       <c r="D26">
         <v>1957</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>324757</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2002</v>
       </c>
@@ -815,13 +895,16 @@
         <v>843.673</v>
       </c>
       <c r="C27">
-        <v>305.16500000000002</v>
+        <v>334660</v>
       </c>
       <c r="D27">
         <v>2004</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>328461</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2003</v>
       </c>
@@ -829,13 +912,16 @@
         <v>1064.52</v>
       </c>
       <c r="C28">
-        <v>306.56900000000002</v>
+        <v>336484</v>
       </c>
       <c r="D28">
         <v>2035</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>323780</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2004</v>
       </c>
@@ -843,13 +929,16 @@
         <v>891.20699999999999</v>
       </c>
       <c r="C29">
-        <v>288.673</v>
+        <v>317059</v>
       </c>
       <c r="D29">
         <v>2048</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>300952</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2005</v>
       </c>
@@ -857,13 +946,16 @@
         <v>745.39100000000008</v>
       </c>
       <c r="C30">
-        <v>263.024</v>
+        <v>288103</v>
       </c>
       <c r="D30">
         <v>2069</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>274389</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2006</v>
       </c>
@@ -871,13 +963,16 @@
         <v>635.85199999999998</v>
       </c>
       <c r="C31">
-        <v>251.459</v>
+        <v>272454</v>
       </c>
       <c r="D31">
         <v>2076</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>266500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2007</v>
       </c>
@@ -885,13 +980,16 @@
         <v>595.50800000000004</v>
       </c>
       <c r="C32">
-        <v>259.93099999999998</v>
+        <v>281250</v>
       </c>
       <c r="D32">
         <v>2054</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>284405</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2008</v>
       </c>
@@ -899,13 +997,16 @@
         <v>827.303</v>
       </c>
       <c r="C33">
-        <v>287.36900000000003</v>
+        <v>316237</v>
       </c>
       <c r="D33">
         <v>2020</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>321322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2009</v>
       </c>
@@ -913,13 +1014,16 @@
         <v>1169.8</v>
       </c>
       <c r="C34">
-        <v>322.63</v>
+        <v>364318</v>
       </c>
       <c r="D34">
         <v>1962</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>365206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2010</v>
       </c>
@@ -927,13 +1031,16 @@
         <v>1380.96</v>
       </c>
       <c r="C35">
-        <v>362.21499999999997</v>
+        <v>421953</v>
       </c>
       <c r="D35">
         <v>1895</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>412065</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2011</v>
       </c>
@@ -941,13 +1048,16 @@
         <v>1316.83</v>
       </c>
       <c r="C36">
-        <v>366.23200000000003</v>
+        <v>441055</v>
       </c>
       <c r="D36">
         <v>1826</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>425550</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2012</v>
       </c>
@@ -955,13 +1065,16 @@
         <v>1223.8100000000002</v>
       </c>
       <c r="C37">
-        <v>358.06599999999997</v>
+        <v>442457</v>
       </c>
       <c r="D37">
         <v>1756</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>431913</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2013</v>
       </c>
@@ -969,13 +1082,16 @@
         <v>1255.6300000000001</v>
       </c>
       <c r="C38">
-        <v>372.54399999999998</v>
+        <v>467633</v>
       </c>
       <c r="D38">
         <v>1701</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>475139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2014</v>
       </c>
@@ -983,13 +1099,16 @@
         <v>994.60699999999997</v>
       </c>
       <c r="C39">
-        <v>419.58699999999999</v>
+        <v>541959</v>
       </c>
       <c r="D39">
         <v>1647</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>553456</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2015</v>
       </c>
@@ -997,13 +1116,16 @@
         <v>2344.69</v>
       </c>
       <c r="C40">
-        <v>335.70400000000001</v>
+        <v>413621</v>
       </c>
       <c r="D40">
         <v>1571</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>408888</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2016</v>
       </c>
@@ -1011,13 +1133,16 @@
         <v>2307.1000000000004</v>
       </c>
       <c r="C41">
-        <v>238.86099999999999</v>
+        <v>278457</v>
       </c>
       <c r="D41">
         <v>1520</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>266608</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2017</v>
       </c>
@@ -1025,13 +1150,16 @@
         <v>1671.89</v>
       </c>
       <c r="C42">
-        <v>152.929</v>
+        <v>166636</v>
       </c>
       <c r="D42">
         <v>1463</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>157240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2018</v>
       </c>
@@ -1039,10 +1167,29 @@
         <v>1186.29</v>
       </c>
       <c r="C43">
-        <v>133.804</v>
+        <v>146433</v>
       </c>
       <c r="D43">
         <v>1421</v>
+      </c>
+      <c r="E43">
+        <v>131650</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E44">
+        <v>149969</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E45">
+        <v>186666</v>
       </c>
     </row>
   </sheetData>
@@ -1051,19 +1198,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888FF985-61AE-764B-ACB4-1C99CD95828C}">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D43"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1076,8 +1223,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1977</v>
       </c>
@@ -1085,13 +1235,16 @@
         <v>132.46</v>
       </c>
       <c r="C2">
-        <v>174.69900000000001</v>
+        <v>240906</v>
       </c>
       <c r="D2">
         <v>355</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>220822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1978</v>
       </c>
@@ -1099,13 +1252,16 @@
         <v>117.4</v>
       </c>
       <c r="C3">
-        <v>193.93</v>
+        <v>260534</v>
       </c>
       <c r="D3">
         <v>366</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>239697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1979</v>
       </c>
@@ -1113,13 +1269,16 @@
         <v>124.39</v>
       </c>
       <c r="C4">
-        <v>189.06399999999999</v>
+        <v>252020</v>
       </c>
       <c r="D4">
         <v>388</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>235975</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1980</v>
       </c>
@@ -1127,13 +1286,16 @@
         <v>172.33</v>
       </c>
       <c r="C5">
-        <v>184.798</v>
+        <v>247466</v>
       </c>
       <c r="D5">
         <v>418</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>240527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1981</v>
       </c>
@@ -1141,13 +1303,16 @@
         <v>188.64000000000004</v>
       </c>
       <c r="C6">
-        <v>211.709</v>
+        <v>302871</v>
       </c>
       <c r="D6">
         <v>450</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>287555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1982</v>
       </c>
@@ -1155,13 +1320,16 @@
         <v>322.90000000000003</v>
       </c>
       <c r="C7">
-        <v>269.20499999999998</v>
+        <v>376994</v>
       </c>
       <c r="D7">
         <v>485</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>333569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1983</v>
       </c>
@@ -1169,13 +1337,16 @@
         <v>450.53</v>
       </c>
       <c r="C8">
-        <v>284.72300000000001</v>
+        <v>395472</v>
       </c>
       <c r="D8">
         <v>528</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>344749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1984</v>
       </c>
@@ -1183,13 +1354,16 @@
         <v>500.72</v>
       </c>
       <c r="C9">
-        <v>287.69900000000001</v>
+        <v>400666</v>
       </c>
       <c r="D9">
         <v>576</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>347180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1985</v>
       </c>
@@ -1197,13 +1371,16 @@
         <v>455.61</v>
       </c>
       <c r="C10">
-        <v>306.01600000000002</v>
+        <v>436257</v>
       </c>
       <c r="D10">
         <v>630</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>377083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1986</v>
       </c>
@@ -1211,13 +1388,16 @@
         <v>412.01</v>
       </c>
       <c r="C11">
-        <v>334.197</v>
+        <v>484999</v>
       </c>
       <c r="D11">
         <v>681</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>422196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1987</v>
       </c>
@@ -1225,13 +1405,16 @@
         <v>384.23</v>
       </c>
       <c r="C12">
-        <v>360.488</v>
+        <v>508411</v>
       </c>
       <c r="D12">
         <v>722</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>454985</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1988</v>
       </c>
@@ -1239,13 +1422,16 @@
         <v>394.9</v>
       </c>
       <c r="C13">
-        <v>388.62</v>
+        <v>510659</v>
       </c>
       <c r="D13">
         <v>749</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>466017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1989</v>
       </c>
@@ -1253,13 +1439,16 @@
         <v>408.03000000000009</v>
       </c>
       <c r="C14">
-        <v>414.85300000000001</v>
+        <v>526359</v>
       </c>
       <c r="D14">
         <v>773</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>486343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1990</v>
       </c>
@@ -1267,13 +1456,16 @@
         <v>417.79</v>
       </c>
       <c r="C15">
-        <v>417.76499999999999</v>
+        <v>521522</v>
       </c>
       <c r="D15">
         <v>805</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>486461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1991</v>
       </c>
@@ -1281,13 +1473,16 @@
         <v>411.54</v>
       </c>
       <c r="C16">
-        <v>378.709</v>
+        <v>473885</v>
       </c>
       <c r="D16">
         <v>843</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>446601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1992</v>
       </c>
@@ -1295,13 +1490,16 @@
         <v>377.07</v>
       </c>
       <c r="C17">
-        <v>339.428</v>
+        <v>430265</v>
       </c>
       <c r="D17">
         <v>884</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>410158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1993</v>
       </c>
@@ -1309,13 +1507,16 @@
         <v>410.83</v>
       </c>
       <c r="C18">
-        <v>306.74299999999999</v>
+        <v>398097</v>
       </c>
       <c r="D18">
         <v>920</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>382899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1994</v>
       </c>
@@ -1323,13 +1524,16 @@
         <v>482.5</v>
       </c>
       <c r="C19">
-        <v>309.815</v>
+        <v>401249</v>
       </c>
       <c r="D19">
         <v>954</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>388969</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1995</v>
       </c>
@@ -1337,13 +1541,16 @@
         <v>401.84999999999997</v>
       </c>
       <c r="C20">
-        <v>321.64</v>
+        <v>402597</v>
       </c>
       <c r="D20">
         <v>978</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>388821</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1996</v>
       </c>
@@ -1351,13 +1558,16 @@
         <v>370.69</v>
       </c>
       <c r="C21">
-        <v>288.09399999999999</v>
+        <v>361454</v>
       </c>
       <c r="D21">
         <v>991</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>345532</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1997</v>
       </c>
@@ -1365,13 +1575,16 @@
         <v>327.23999999999995</v>
       </c>
       <c r="C22">
-        <v>242.58500000000001</v>
+        <v>302929</v>
       </c>
       <c r="D22">
         <v>1008</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>293694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1998</v>
       </c>
@@ -1379,13 +1592,16 @@
         <v>255.24999999999997</v>
       </c>
       <c r="C23">
-        <v>203.45400000000001</v>
+        <v>245753</v>
       </c>
       <c r="D23">
         <v>1017</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>247246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1999</v>
       </c>
@@ -1393,13 +1609,16 @@
         <v>236.6</v>
       </c>
       <c r="C24">
-        <v>179.113</v>
+        <v>214551</v>
       </c>
       <c r="D24">
         <v>1020</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>220957</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2000</v>
       </c>
@@ -1407,13 +1626,16 @@
         <v>223.76</v>
       </c>
       <c r="C25">
-        <v>160.47900000000001</v>
+        <v>190885</v>
       </c>
       <c r="D25">
         <v>1012</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>194687</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2001</v>
       </c>
@@ -1421,13 +1643,16 @@
         <v>209.37</v>
       </c>
       <c r="C26">
-        <v>149.98099999999999</v>
+        <v>175240</v>
       </c>
       <c r="D26">
         <v>966</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>175784</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2002</v>
       </c>
@@ -1435,13 +1660,16 @@
         <v>173.99</v>
       </c>
       <c r="C27">
-        <v>146.15700000000001</v>
+        <v>165709</v>
       </c>
       <c r="D27">
         <v>991</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>167020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2003</v>
       </c>
@@ -1449,13 +1677,16 @@
         <v>162.92999999999998</v>
       </c>
       <c r="C28">
-        <v>150.91</v>
+        <v>165570</v>
       </c>
       <c r="D28">
         <v>997</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>165756</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2004</v>
       </c>
@@ -1463,13 +1694,16 @@
         <v>184.12</v>
       </c>
       <c r="C29">
-        <v>157.36000000000001</v>
+        <v>171104</v>
       </c>
       <c r="D29">
         <v>1016</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>166849</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2005</v>
       </c>
@@ -1477,13 +1711,16 @@
         <v>222.53</v>
       </c>
       <c r="C30">
-        <v>153.73599999999999</v>
+        <v>166219</v>
       </c>
       <c r="D30">
         <v>1065</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>158075</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2006</v>
       </c>
@@ -1491,13 +1728,16 @@
         <v>240.94</v>
       </c>
       <c r="C31">
-        <v>138.648</v>
+        <v>152138</v>
       </c>
       <c r="D31">
         <v>1118</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>141916</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2007</v>
       </c>
@@ -1505,13 +1745,16 @@
         <v>213.87</v>
       </c>
       <c r="C32">
-        <v>120.645</v>
+        <v>133144</v>
       </c>
       <c r="D32">
         <v>1155</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>124747</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2008</v>
       </c>
@@ -1519,13 +1762,16 @@
         <v>212.04999999999998</v>
       </c>
       <c r="C33">
-        <v>107.679</v>
+        <v>118934</v>
       </c>
       <c r="D33">
         <v>1173</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>116691</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2009</v>
       </c>
@@ -1533,13 +1779,16 @@
         <v>212.23</v>
       </c>
       <c r="C34">
-        <v>110.16200000000001</v>
+        <v>124955</v>
       </c>
       <c r="D34">
         <v>1170</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>126048</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2010</v>
       </c>
@@ -1547,13 +1796,16 @@
         <v>289.64</v>
       </c>
       <c r="C35">
-        <v>141.45699999999999</v>
+        <v>162165</v>
       </c>
       <c r="D35">
         <v>1164</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>164317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2011</v>
       </c>
@@ -1561,13 +1813,16 @@
         <v>339.72999999999996</v>
       </c>
       <c r="C36">
-        <v>162.49199999999999</v>
+        <v>190668</v>
       </c>
       <c r="D36">
         <v>1156</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>186628</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2012</v>
       </c>
@@ -1575,13 +1830,16 @@
         <v>359.92</v>
       </c>
       <c r="C37">
-        <v>170.43199999999999</v>
+        <v>210816</v>
       </c>
       <c r="D37">
         <v>1136</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>198720</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2013</v>
       </c>
@@ -1589,13 +1847,16 @@
         <v>385.46999999999991</v>
       </c>
       <c r="C38">
-        <v>172.97900000000001</v>
+        <v>219493</v>
       </c>
       <c r="D38">
         <v>1112</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>205243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2014</v>
       </c>
@@ -1603,13 +1864,16 @@
         <v>298.53000000000009</v>
       </c>
       <c r="C39">
-        <v>165.10400000000001</v>
+        <v>219628</v>
       </c>
       <c r="D39">
         <v>1074</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>213549</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2015</v>
       </c>
@@ -1617,13 +1881,16 @@
         <v>260.89</v>
       </c>
       <c r="C40">
-        <v>119.173</v>
+        <v>152560</v>
       </c>
       <c r="D40">
         <v>1014</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>156531</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2016</v>
       </c>
@@ -1631,13 +1898,16 @@
         <v>282.38</v>
       </c>
       <c r="C41">
-        <v>100.203</v>
+        <v>120170</v>
       </c>
       <c r="D41">
         <v>966</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>125791</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2017</v>
       </c>
@@ -1645,13 +1915,16 @@
         <v>351.85</v>
       </c>
       <c r="C42">
-        <v>84.676199999999994</v>
+        <v>90748.9</v>
       </c>
       <c r="D42">
         <v>923</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>89922.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2018</v>
       </c>
@@ -1659,10 +1932,29 @@
         <v>325.54000000000002</v>
       </c>
       <c r="C43">
-        <v>75.781899999999993</v>
+        <v>79446.3</v>
       </c>
       <c r="D43">
         <v>0</v>
+      </c>
+      <c r="E43">
+        <v>71879.600000000006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E44">
+        <v>69588.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E45">
+        <v>69262.5</v>
       </c>
     </row>
   </sheetData>
@@ -1671,19 +1963,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821929F5-19A9-8141-AF93-BF465999D3E5}">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1696,8 +1988,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1977</v>
       </c>
@@ -1710,8 +2005,11 @@
       <c r="D2">
         <v>0.76300000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1207580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1978</v>
       </c>
@@ -1724,8 +2022,11 @@
       <c r="D3">
         <v>0.877</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>377556</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1979</v>
       </c>
@@ -1738,8 +2039,11 @@
       <c r="D4">
         <v>0.96699999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>369733</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1980</v>
       </c>
@@ -1752,8 +2056,11 @@
       <c r="D5">
         <v>0.877</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>624014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1981</v>
       </c>
@@ -1766,8 +2073,11 @@
       <c r="D6">
         <v>0.73499999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>689951</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1982</v>
       </c>
@@ -1780,8 +2090,11 @@
       <c r="D7">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>756252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1983</v>
       </c>
@@ -1794,8 +2107,11 @@
       <c r="D8">
         <v>0.69699999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>538912</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1984</v>
       </c>
@@ -1808,8 +2124,11 @@
       <c r="D9">
         <v>0.88400000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>709138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1985</v>
       </c>
@@ -1822,8 +2141,11 @@
       <c r="D10">
         <v>1.17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>886695</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1986</v>
       </c>
@@ -1836,8 +2158,11 @@
       <c r="D11">
         <v>0.98799999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>499375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1987</v>
       </c>
@@ -1850,8 +2175,11 @@
       <c r="D12">
         <v>1.0229999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>588083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1988</v>
       </c>
@@ -1864,8 +2192,11 @@
       <c r="D13">
         <v>1.179</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>597962</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1989</v>
       </c>
@@ -1878,8 +2209,11 @@
       <c r="D14">
         <v>1.028</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>632229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1990</v>
       </c>
@@ -1892,8 +2226,11 @@
       <c r="D15">
         <v>0.90400000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>749185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1991</v>
       </c>
@@ -1906,8 +2243,11 @@
       <c r="D16">
         <v>1.0469999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>444758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1992</v>
       </c>
@@ -1920,8 +2260,11 @@
       <c r="D17">
         <v>0.94399999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>385255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1993</v>
       </c>
@@ -1934,8 +2277,11 @@
       <c r="D18">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>309854</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1994</v>
       </c>
@@ -1948,8 +2294,11 @@
       <c r="D19">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>347856</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1995</v>
       </c>
@@ -1962,8 +2311,11 @@
       <c r="D20">
         <v>0.82899999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>438067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1996</v>
       </c>
@@ -1976,8 +2328,11 @@
       <c r="D21">
         <v>0.82299999999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>309470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1997</v>
       </c>
@@ -1990,8 +2345,11 @@
       <c r="D22">
         <v>1.077</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>293505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1998</v>
       </c>
@@ -2004,8 +2362,11 @@
       <c r="D23">
         <v>1.2969999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>272155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1999</v>
       </c>
@@ -2018,8 +2379,11 @@
       <c r="D24">
         <v>1.345</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>366527</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2000</v>
       </c>
@@ -2032,8 +2396,11 @@
       <c r="D25">
         <v>1.766</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>439377</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2001</v>
       </c>
@@ -2046,8 +2413,11 @@
       <c r="D26">
         <v>1.1220000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>250745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2002</v>
       </c>
@@ -2060,8 +2430,11 @@
       <c r="D27">
         <v>1.0469999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>193147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2003</v>
       </c>
@@ -2074,8 +2447,11 @@
       <c r="D28">
         <v>0.93799999999999994</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>244348</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2004</v>
       </c>
@@ -2088,8 +2464,11 @@
       <c r="D29">
         <v>1.0129999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>307845</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2005</v>
       </c>
@@ -2102,8 +2481,11 @@
       <c r="D30">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>420358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2006</v>
       </c>
@@ -2116,8 +2498,11 @@
       <c r="D31">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>686754</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2007</v>
       </c>
@@ -2130,8 +2515,11 @@
       <c r="D32">
         <v>0.69799999999999995</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>443195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2008</v>
       </c>
@@ -2144,8 +2532,11 @@
       <c r="D33">
         <v>0.69299999999999995</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>651882</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2009</v>
       </c>
@@ -2158,8 +2549,11 @@
       <c r="D34">
         <v>0.503</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>391813</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2010</v>
       </c>
@@ -2172,8 +2566,11 @@
       <c r="D35">
         <v>0.495</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>506839</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2011</v>
       </c>
@@ -2186,8 +2583,11 @@
       <c r="D36">
         <v>0.624</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>655108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2012</v>
       </c>
@@ -2200,8 +2600,11 @@
       <c r="D37">
         <v>0.753</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>1215110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2013</v>
       </c>
@@ -2214,8 +2617,11 @@
       <c r="D38">
         <v>0.73499999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>638080</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2014</v>
       </c>
@@ -2228,8 +2634,11 @@
       <c r="D39">
         <v>0.63800000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>211074</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2015</v>
       </c>
@@ -2242,8 +2651,11 @@
       <c r="D40">
         <v>0.43099999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>260163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2016</v>
       </c>
@@ -2256,8 +2668,11 @@
       <c r="D41">
         <v>0.61399999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>168038</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2017</v>
       </c>
@@ -2270,8 +2685,11 @@
       <c r="D42">
         <v>0.436</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>246044</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2018</v>
       </c>
@@ -2283,6 +2701,25 @@
       </c>
       <c r="D43">
         <v>0</v>
+      </c>
+      <c r="E43">
+        <v>389895</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E44">
+        <v>399011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E45">
+        <v>463705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 18.5.1. Halibut runs
Updated combine data and included halibut models aaf, coast, survey
</commit_message>
<xml_diff>
--- a/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_biomass_estimate.xlsx
+++ b/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_biomass_estimate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380" activeTab="2"/>
+    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="1" r:id="rId1"/>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1202,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1934,9 +1934,7 @@
       <c r="C43">
         <v>79446.3</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
+      <c r="D43"/>
       <c r="E43">
         <v>71879.600000000006</v>
       </c>
@@ -1966,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2699,9 +2697,7 @@
       <c r="C43">
         <v>0.67705000000000004</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
+      <c r="D43"/>
       <c r="E43">
         <v>389895</v>
       </c>

</xml_diff>